<commit_message>
Added new triangulation2 script
</commit_message>
<xml_diff>
--- a/Test_Results/Test_Results_1/toa_cal.xlsx
+++ b/Test_Results/Test_Results_1/toa_cal.xlsx
@@ -463,22 +463,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0009112048919340322</v>
+        <v>0.9112048919340322</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001133786848072562</v>
+        <v>1.133786848072562</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0001126721327937182</v>
+        <v>0.1126721327937182</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0009070294784580499</v>
+        <v>0.9070294784580499</v>
       </c>
       <c r="F2" t="n">
-        <v>0.001139435185830596</v>
+        <v>1.139435185830596</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0001133786848072562</v>
+        <v>0.1133786848072562</v>
       </c>
     </row>
     <row r="3">
@@ -486,22 +486,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.001516781676858299</v>
+        <v>-0.4402577480568004</v>
       </c>
       <c r="C3" t="n">
-        <v>0.001428571428571429</v>
+        <v>-0.36281179138322</v>
       </c>
       <c r="D3" t="n">
-        <v>-2.780478836149347e-05</v>
+        <v>0.1028323251606915</v>
       </c>
       <c r="E3" t="n">
-        <v>0.001519274376417233</v>
+        <v>-0.4308390022675737</v>
       </c>
       <c r="F3" t="n">
-        <v>0.001434884998724698</v>
+        <v>-0.3662529298129745</v>
       </c>
       <c r="G3" t="n">
-        <v>-2.267573696145125e-05</v>
+        <v>0.1133786848072562</v>
       </c>
     </row>
     <row r="4">
@@ -509,22 +509,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.001413437127069169</v>
+        <v>-2.031350183375844</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.001111111111111111</v>
+        <v>-2.448979591836735</v>
       </c>
       <c r="D4" t="n">
-        <v>0.000958924527989136</v>
+        <v>-1.253243669098878</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.001405895691609977</v>
+        <v>-2.040816326530612</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.001130043548555386</v>
+        <v>-2.444198566859693</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0009750566893424037</v>
+        <v>-1.26984126984127</v>
       </c>
     </row>
     <row r="5">
@@ -532,22 +532,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0005427231402663474</v>
+        <v>-0.002692718193406324</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.0002494331065759637</v>
+        <v>-0.2040816326530612</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0006046514341196923</v>
+        <v>-0.1855199464135275</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0005442176870748299</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.0002657490005518468</v>
+        <v>-0.1878768028333454</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.0005895691609977325</v>
+        <v>-0.18140589569161</v>
       </c>
     </row>
     <row r="6">
@@ -555,22 +555,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.000660511221216038</v>
+        <v>1.541215953830037</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001201814058956916</v>
+        <v>1.927437641723356</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0003138240679746371</v>
+        <v>0.1231218379758774</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0006575963718820862</v>
+        <v>1.541950113378685</v>
       </c>
       <c r="F6" t="n">
-        <v>0.001204305842814798</v>
+        <v>1.945556573671575</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0003174603174603175</v>
+        <v>0.1133786848072562</v>
       </c>
     </row>
     <row r="7">
@@ -578,22 +578,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.000942156936939036</v>
+        <v>-0.3802581138671877</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0006349206349206349</v>
+        <v>0.18140589569161</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0001632543943753059</v>
+        <v>0.7815463054709451</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0009297052154195011</v>
+        <v>-0.3854875283446712</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0006354360378626705</v>
+        <v>0.1838007771989899</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.00018140589569161</v>
+        <v>0.7709750566893424</v>
       </c>
     </row>
     <row r="8">
@@ -601,22 +601,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0006711348559926249</v>
+        <v>0.5145133491967829</v>
       </c>
       <c r="C8" t="n">
-        <v>-6.802721088435374e-05</v>
+        <v>0.453514739229025</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0005021297036625328</v>
+        <v>-0.04511345882168556</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0006802721088435374</v>
+        <v>0.5215419501133787</v>
       </c>
       <c r="F8" t="n">
-        <v>-6.11665199638158e-05</v>
+        <v>0.449486283507921</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.0004988662131519275</v>
+        <v>-0.04535147392290249</v>
       </c>
     </row>
     <row r="9">
@@ -624,22 +624,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.001586890114503978</v>
+        <v>0.4907005132262501</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0009523809523809524</v>
+        <v>1.224489795918367</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.0002353042992312687</v>
+        <v>0.4794669711284663</v>
       </c>
       <c r="E9" t="n">
-        <v>0.001587301587301587</v>
+        <v>0.4988662131519275</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0009489185067925591</v>
+        <v>1.220539079278846</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.0002267573696145125</v>
+        <v>0.4761904761904762</v>
       </c>
     </row>
     <row r="10">
@@ -647,22 +647,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.001479242589904325</v>
+        <v>1.165374245474661</v>
       </c>
       <c r="C10" t="n">
-        <v>0.001179138321995465</v>
+        <v>2.244897959183673</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0001113607302424286</v>
+        <v>0.3733966858293393</v>
       </c>
       <c r="E10" t="n">
-        <v>0.001496598639455782</v>
+        <v>1.179138321995465</v>
       </c>
       <c r="F10" t="n">
-        <v>0.001174680052019589</v>
+        <v>2.245223706833127</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.0001133786848072562</v>
+        <v>0.3854875283446712</v>
       </c>
     </row>
     <row r="11">
@@ -670,22 +670,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.001726122954404271</v>
+        <v>0.8777519492556363</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.002018140589569161</v>
+        <v>0.4308390022675737</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.0008027147608834736</v>
+        <v>-0.2530379391380345</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.001723356009070295</v>
+        <v>0.8843537414965986</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.002008098387831892</v>
+        <v>0.4345807984913791</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.0008163265306122449</v>
+        <v>-0.2494331065759637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>